<commit_message>
worked on everything but the flicker
</commit_message>
<xml_diff>
--- a/conditions/MIL_teen_prac.xlsx
+++ b/conditions/MIL_teen_prac.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Katie/Dropbox/LearningStudy/Teen_MIL/conditions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katharinaseitz/Documents/projects/RL-scancamp/conditions/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4FF57E-C984-B849-9515-AAAB7B0CA187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="1260" windowWidth="22160" windowHeight="10360" tabRatio="500"/>
+    <workbookView xWindow="3440" yWindow="1260" windowWidth="22160" windowHeight="10360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,12 +30,6 @@
     <t>Trials</t>
   </si>
   <si>
-    <t>LeftImage</t>
-  </si>
-  <si>
-    <t>RightImage</t>
-  </si>
-  <si>
     <t>images/prac1.png</t>
   </si>
   <si>
@@ -42,12 +37,18 @@
   </si>
   <si>
     <t>PracCorrect</t>
+  </si>
+  <si>
+    <t>leftImgPath</t>
+  </si>
+  <si>
+    <t>rightImgPath</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -88,6 +89,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -355,11 +359,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -369,13 +373,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -383,10 +387,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -397,10 +401,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -411,10 +415,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -425,10 +429,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -439,10 +443,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>1</v>

</xml_diff>

<commit_message>
worked on the practice
</commit_message>
<xml_diff>
--- a/conditions/MIL_teen_prac.xlsx
+++ b/conditions/MIL_teen_prac.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katharinaseitz/Documents/projects/RL-scancamp/conditions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4FF57E-C984-B849-9515-AAAB7B0CA187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44C4522-3829-6D40-B6BC-9C2B550A647D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="1260" windowWidth="22160" windowHeight="10360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3440" yWindow="1260" windowWidth="25980" windowHeight="14460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t>Trials</t>
   </si>
@@ -36,13 +36,22 @@
     <t>images/prac2.png</t>
   </si>
   <si>
-    <t>PracCorrect</t>
-  </si>
-  <si>
     <t>leftImgPath</t>
   </si>
   <si>
     <t>rightImgPath</t>
+  </si>
+  <si>
+    <t>PracCorrectScan</t>
+  </si>
+  <si>
+    <t>PracCorrectPilot</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>right</t>
   </si>
 </sst>
 </file>
@@ -360,29 +369,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="24.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -395,8 +410,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -409,8 +427,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -423,8 +444,11 @@
       <c r="D4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -437,8 +461,11 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -450,6 +477,9 @@
       </c>
       <c r="D6">
         <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>